<commit_message>
Update Level 2 screen
2단계화면 최종
</commit_message>
<xml_diff>
--- a/master/website/static/datatemplates/itempermanucost.xlsx
+++ b/master/website/static/datatemplates/itempermanucost.xlsx
@@ -429,12 +429,12 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>int(11)</t>
+          <t>varchar(50)</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>varchar(50)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -444,54 +444,54 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>int(11)</t>
+          <t>varchar(50)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>int(11)</t>
+          <t>int(255)</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>int(255)</t>
+          <t>int(6)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>ID (입력x)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>co_id</t>
+          <t>법인코드</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ipmc_ym</t>
+          <t>bom코드</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ipmc_version</t>
+          <t>계정코드</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>moitem_id</t>
+          <t>version코드</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>itemaccnt_id</t>
+          <t>금액</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ipmc_cost</t>
+          <t>년월 ex) 200001</t>
         </is>
       </c>
     </row>

</xml_diff>